<commit_message>
Committed on 01:03:2018:11:50:00PM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Episerver_Campaign_Validation_500.xlsx
+++ b/data/Episerver_Campaign_Validation_500.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\workspace\Ameex_Marketing_Team\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="8385" windowWidth="20385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8385"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="1002">
   <si>
     <t>Email ID</t>
   </si>
@@ -2323,20 +2328,1210 @@
   </si>
   <si>
     <t>apaul@lakewood.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>aperry@primr.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>apeterson@sigmarep.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>apeugh@lottmarketing.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>apickard@sudbury.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>apietrala@njcu.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>arcurij@nwmedstar.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>areinstein@showcase.ca is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if arleen.b@peimedia.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>armstrongr@warhol.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>arosen@translab.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>arseneau.hughes@universalsales.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>art@lakecountryfinancialplanning.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>arthur@fmbadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>arubio@usfca.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>arussell@kuyper.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>arwoods1@michigan.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>asaita@isc2.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>aschilling@ktvn.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if aschneider@maritime-ins.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>asegall@wga.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>asenn@aseadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>asetterlund@loram.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ashley.royal@logisticssupply.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Ashley@Prescott500.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Ashley@ZogSports.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>asickbert01@hamline.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>aspeicher@aau.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>astallings@hydrolox.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if aterrillion@astho.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>atrehan@commscope.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>audra.early@kindredhealthcare.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>aurelias@orbuscompany.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Austin.Winkleman@swic.edu is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>award@maximphysicians.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if aweddle@hivma.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>aweiss@sigadvisors.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if aweissmann@travelweekly.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>awilliams@galenefinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>awilliams@greatlakesfinancialservices.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>awolle@advancedcirculatory.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>azaffa@ocm.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>b.patrick@moreheadstate.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>BaderV@adea.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bahner@wipga.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ballen@aom.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ballen@olivet.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>balvarado@thestrategypartnersinc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if barb.biernat@tottengroup.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>barbara.callahan@cit.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if barbara.clough@newportgroup.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if barbara.williams@shawmedia.ca
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>barbaram@astro.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>barry.canipe@carestream.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>barry.toiv@aau.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>barrymcbride@suncornerstone.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if batchason@westgablesrehabhospital.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbaldwin@ncb.coop is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbarker@namb.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>BBarnes@theBDX.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbecher@authorsolutions.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbeemer@attorneygeneral.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbennett@dfginv.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bberndt@volt.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbettmann@ccu.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbishop@davidjeremiah.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bboon@carf.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bborden@compasscapitalweb.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbradin@lesley.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbrinson@egov.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbriscoe@capital.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbrodbeck@dbgfinancialgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bburkes@kkg.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bburrell@pequotmuseum.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbutler@zoll.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bbutz@maxhealth.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bcameron@iienet.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bcarville@geneseevalleytrust.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if BColeman@mbci.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>beachamdm@wofford.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>becky.wilmot@anchor-wealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>becky.woolman@woolman.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>belisle.jason@irvingcrane.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>belliott@authorsolutions.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ben.dempsey@riverbendtitlellc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ben.julianel@tfgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Ben.Koley@FinancialVisionsLLC.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ben.schilens@ektron.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ben.simpson@cablecam.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bennett.weston@kenthomes.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bensign@bicsi.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>berkel@cancerpreventioninstitute.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bernard.delomenie@crowehorwath.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bernd.wellhaus@bakelite.de
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bert.clark@infrastructureontario.ca is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>beth.montgomery@kindredhealthcare.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>beth.rampelberg@nsca.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>betty.custer@LFG.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>betty.sullivan@rogers.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bevans@techcu.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bfields@rhodeislandhousing.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bgamba@jewelersboard.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bghering@windsorplywood.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bgill@dana.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bhaley@saberdentalstudio.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bhilton@inseroequipment.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bhm@wfu.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bhusselbee@valassis.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bill.butz@maximwellness.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bill.hubbard@harrisonmedical.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bill.lloyd@lpl.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bill.perry@perdue.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bill@wsga.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bissone@nwmedstar.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bitell@rotarylift.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bjarrell@umaryland.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bjohns@volt.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bjones@waukeshacounty.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bjordan@fhnc.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bjordan@firsthorizon.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bjulien@bicsi.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bking@archinsurance.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>BKivovit@militarycars.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>blaine@rfsny.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>blake.schinto@progressivetitle.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>blakleyj@chesterfield.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>blewis@ufadvisors.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>blloyd@qualitrolcorp.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>blmayea@sc4.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bmete@brooksequipment.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bmiller@valleyhealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bmimura@calendow.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bmonbarren@injuryboard.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bmoore@iclfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bmorena@jimmyjohns.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bnixon@ctlgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>boardmember@aiaa.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bob.chalker@nace.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bob.fair@teradata.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bob.king@aosepc.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bob.milner@st-johns.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bob.narracci@eaglecounty.us is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bob_robuck@centralbancompany.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bobbrown@uclfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bobs@syaeng.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bobw@hobbytown.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>boby@dsidoorservices.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bodenlosk@carnegiemnh.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Bonnie.Owens@staffcare.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bostrowski@utilimaster.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>boychick888@gmail.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bpatton@vantagepartners.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bpfeifer@bonddesk.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bphess@hesssegal.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>BPleasant@UCStrategies.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bpowell@brpcpas.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brad.little@selectphysicaltherapy.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brad@bauerdental.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brad@champlinandassociates.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brad@kercheville.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brad@kipinvest.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brad@midwestsecureretirement.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bradley.joseph@perrigo.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bradley@hendrix.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bradp@jvcpa.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brady@sternempire.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brandie.belangeri@firstcaliforniaescrow.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>BrandiG@PathwayEstate.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brandon@ascendorwealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brant@steward-wealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brayd@prisco.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bredman@securianadvisorsnw.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Brenda.Jeffers@stjohnscollegespringfield.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brenda.kostelak@compasscapitalweb.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brenda@ncpga.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brent@bear-stone.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bret.preston@cambridgesecure.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bret@sbgfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.connely@spartanerv.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.jepson@ohiohealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Brian.Kilduff@viewpointe.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.longbons@lpl.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.love@owb.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.mccloskey@amnhealthcare.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.peters@medtravelers.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if brian.reardon@st-johns.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.rich@cmsenergy.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.salerno@bsee.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.shields@deltadentalva.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.simpson@netmatrix.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.zulli@trgc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian@advisorspfg.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian@brybeck.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian@downeastglass.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian@educyber.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian@gpsfinancialadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian@melnickrosenbaum.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian@summitplanninggroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>briana.larkin@rhf.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brianf@gjcity.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brichardson@judsonu.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brisser@pci.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brittany.bethune@nygard.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>broberts@financialguide.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brosmj@jea.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bruce.kendrick@veyance.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bruce.walthers@frontrange.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bruce_redfield@hsbct.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brucea@canogawealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if Bruss@QMACS.COM
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bryan.cossette@nov.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bryan.hackett@proequities.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bryan.neary@cso.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bryan@msamsa.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bryan_goodman@americanchemistry.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>BSehlhorst@REDICincinnati.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bsellers@wsfsbank.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bsigmon@vidanthealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bsmith@westcoastfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if BSnyder@marcusa.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bswift@tcms.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if burke@reinsurance.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bwinters@tompkinsfinancialadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bwolters@kentwa.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bwriter@financialguide.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>c.chen@esmarttax.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>c.denny@angelusplaza.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cafriffith@atriummedcenter.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if cahoffman@clearperspectivesllc.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cain.aaron@veyance.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>caren.madsen@boem.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carl.hafele@lanieram.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carla.bourque@alc.ca is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carlosdacruz@miamibeachfl.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>caro@hendrix.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carol.burke@nursezone.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if carol.gawrylash@tottengroup.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if carol.lichon@sarasotacountyschools.net
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>caroleb@nebmed.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carolr@moaa.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carolyn.boston@pgcps.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carolyn.wagner@carestreamhealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carolyn@weatherlyassetmgt.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if carrie.catlin@perdue.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carrie.houser@woolman.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Carrie.Toth@mhcc.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>carriewright@guidegrp.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Caryng@pgane.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>catherine.beaman@nursechoice.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>catherine.rea@seattlechildrens.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>catherine.richardson@ciab.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>catherine@advancedautobat.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cattan@aisc.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if cbanton@physiocontrol.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if cbarker@promnetwork.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cbarr@smithassoc.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if cbauer@anchorbank.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cbenton@healthtech.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cbielecki@foundationsfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cblanks@maseniorcare.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if cbosselaar@phocuswright.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cbrayton@garaga.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cbrewer@uscupstate.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ccarter@transitionresources.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Cciervo@monmouth.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>CClark@FLmedical.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ccoltrane@abilityexperience.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ccornell@johnsonoutdoors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ccrispen@sifma.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ccundey@johnsonoutdoors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cday@frontlinemarketing.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cdemars@the-alliance.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cdjohnson@coefed.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cdrury@cost.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cecilia.perez@milliman.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cecooper@umc.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cedavis@therulewm.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cedwards@carrollcc.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cehassinger@sfgweb.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>celder@royalgrouptech.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if ceo@kaplancollege.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cfrazier@frontlinemarketing.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if cfritsche@williamcharlesconstruction.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cgmiller@kiesskraft.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cgrosse@greaterlouisville.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chackley@foundationsfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chad.berger@tsi.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Chad.Boreman@fdgonline.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chad.couser@safenet-inc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chad@iosolutions.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chad@ledgestonecapital.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chadcartier@pillarplanfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chadnoble@cebertwealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chammond@ahlef.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chandrafrederick@polk-county.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chapdelaine@hood.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>charles.hinrichs@regalbeloit.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>charlie.aleshire@harrisonmedical.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Charlie@PrismFG.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>charmm@jea.com is
 a valid deliverable e-mail box address.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2362,70 +3557,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2435,83 +3569,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2520,31 +3579,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2556,156 +3591,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2728,270 +3643,46 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="57">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="43">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="44">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="41">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="6" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="17" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="22" fontId="19" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="21" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="15" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="15" fontId="22" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="20" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="7" numFmtId="0"/>
+  <cellStyleXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="57">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="9">
+    <cellStyle name="60% - Accent1 2" xfId="6"/>
+    <cellStyle name="60% - Accent2 2" xfId="7"/>
+    <cellStyle name="60% - Accent3 2" xfId="3"/>
+    <cellStyle name="60% - Accent4 2" xfId="5"/>
     <cellStyle name="60% - Accent5 2" xfId="1"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="2"/>
-    <cellStyle builtinId="3" name="Comma" xfId="3"/>
-    <cellStyle builtinId="4" name="Currency" xfId="4"/>
-    <cellStyle builtinId="6" name="Comma[0]" xfId="5"/>
-    <cellStyle builtinId="5" name="Percent" xfId="6"/>
-    <cellStyle builtinId="7" name="Currency[0]" xfId="7"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="8"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="9"/>
-    <cellStyle builtinId="10" name="Note" xfId="10"/>
-    <cellStyle name="60% - Accent6 2" xfId="11"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="12"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="13"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="14"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="15"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="16"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="17"/>
-    <cellStyle builtinId="15" name="Title" xfId="18"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="19"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="20"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="21"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="22"/>
-    <cellStyle builtinId="20" name="Input" xfId="23"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="24"/>
-    <cellStyle builtinId="26" name="Good" xfId="25"/>
-    <cellStyle builtinId="21" name="Output" xfId="26"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="27"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="28"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="29"/>
-    <cellStyle builtinId="25" name="Total" xfId="30"/>
-    <cellStyle name="60% - Accent3 2" xfId="31"/>
-    <cellStyle builtinId="27" name="Bad" xfId="32"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="33"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="34"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="35"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="36"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="37"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="38"/>
-    <cellStyle name="Title 2" xfId="39"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="40"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="41"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="42"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="43"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="44"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="45"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="46"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="47"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="48"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="49"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="50"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="51"/>
-    <cellStyle name="60% - Accent4 2" xfId="52"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="53"/>
-    <cellStyle name="60% - Accent1 2" xfId="54"/>
-    <cellStyle name="60% - Accent2 2" xfId="55"/>
-    <cellStyle name="Neutral 2" xfId="56"/>
+    <cellStyle name="60% - Accent6 2" xfId="2"/>
+    <cellStyle name="Neutral 2" xfId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title 2" xfId="4"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3000,10 +3691,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -3167,21 +3858,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -3198,7 +3889,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -3252,18 +3943,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
-  <dimension ref="A1:C501"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A475" workbookViewId="0">
+      <selection activeCell="D483" sqref="D483"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.8571428571429" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="98.7142857142857" collapsed="true"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="109.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4886,1798 +5576,2395 @@
       <c r="A203" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B203" s="2"/>
+      <c r="B203" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B204" s="2"/>
+      <c r="B204" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B205" s="2"/>
+      <c r="B205" s="2" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B206" s="2"/>
+      <c r="B206" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B207" s="2"/>
+      <c r="B207" s="2" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B208" s="2"/>
+      <c r="B208" s="2" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B209" s="2"/>
+      <c r="B209" s="2" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B210" s="2"/>
+      <c r="B210" s="2" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B211" s="2"/>
+      <c r="B211" s="2" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B212" s="2"/>
+      <c r="B212" s="2" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B213" s="2"/>
+      <c r="B213" s="2" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B214" s="2"/>
+      <c r="B214" s="2" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B215" s="2"/>
+      <c r="B215" s="2" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B216" s="2"/>
+      <c r="B216" s="2" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B217" s="2"/>
+      <c r="B217" s="2" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B218" s="2"/>
+      <c r="B218" s="2" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B219" s="2"/>
+      <c r="B219" s="2" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B220" s="2"/>
+      <c r="B220" s="2" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B221" s="2"/>
+      <c r="B221" s="2" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B222" s="2"/>
+      <c r="B222" s="2" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B223" s="2"/>
+      <c r="B223" s="2" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B224" s="2"/>
+      <c r="B224" s="2" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B225" s="2"/>
+      <c r="B225" s="2" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B226" s="2"/>
+      <c r="B226" s="2" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B227" s="2"/>
+      <c r="B227" s="2" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B228" s="2"/>
+      <c r="B228" s="2" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B229" s="2"/>
+      <c r="B229" s="2" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B230" s="2"/>
+      <c r="B230" s="2" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B231" s="2"/>
+      <c r="B231" s="2" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B232" s="2"/>
+      <c r="B232" s="2" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B233" s="2"/>
+      <c r="B233" s="2" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B234" s="2"/>
+      <c r="B234" s="2" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B235" s="2"/>
+      <c r="B235" s="2" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B236" s="2"/>
+      <c r="B236" s="2" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B237" s="2"/>
+      <c r="B237" s="2" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B238" s="2"/>
+      <c r="B238" s="2" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B239" s="2"/>
+      <c r="B239" s="2" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B240" s="2"/>
+      <c r="B240" s="2" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B241" s="2"/>
+      <c r="B241" s="2" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B242" s="2"/>
+      <c r="B242" s="2" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B243" s="2"/>
+      <c r="B243" s="2" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B244" s="2"/>
+      <c r="B244" s="2" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B245" s="2"/>
+      <c r="B245" s="2" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B246" s="2"/>
+      <c r="B246" s="2" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B247" s="2"/>
+      <c r="B247" s="2" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B248" s="2"/>
+      <c r="B248" s="2" t="s">
+        <v>748</v>
+      </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B249" s="2"/>
+      <c r="B249" s="2" t="s">
+        <v>749</v>
+      </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B250" s="2"/>
+      <c r="B250" s="2" t="s">
+        <v>750</v>
+      </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B251" s="2"/>
+      <c r="B251" s="2" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B252" s="2"/>
+      <c r="B252" s="2" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B253" s="2"/>
+      <c r="B253" s="2" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B254" s="2"/>
+      <c r="B254" s="2" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B255" s="2"/>
+      <c r="B255" s="2" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B256" s="2"/>
+      <c r="B256" s="2" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B257" s="2"/>
+      <c r="B257" s="2" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B258" s="2"/>
+      <c r="B258" s="2" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B259" s="2"/>
+      <c r="B259" s="2" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B260" s="2"/>
+      <c r="B260" s="2" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B261" s="2"/>
+      <c r="B261" s="2" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B262" s="2"/>
+      <c r="B262" s="2" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B263" s="2"/>
+      <c r="B263" s="2" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B264" s="2"/>
+      <c r="B264" s="2" t="s">
+        <v>764</v>
+      </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B265" s="2"/>
+      <c r="B265" s="2" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B266" s="2"/>
+      <c r="B266" s="2" t="s">
+        <v>766</v>
+      </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B267" s="2"/>
+      <c r="B267" s="2" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B268" s="2"/>
+      <c r="B268" s="2" t="s">
+        <v>768</v>
+      </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B269" s="2"/>
+      <c r="B269" s="2" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B270" s="2"/>
+      <c r="B270" s="2" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B271" s="2"/>
+      <c r="B271" s="2" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B272" s="2"/>
+      <c r="B272" s="2" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B273" s="2"/>
+      <c r="B273" s="2" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B274" s="2"/>
+      <c r="B274" s="2" t="s">
+        <v>774</v>
+      </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B275" s="2"/>
+      <c r="B275" s="2" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B276" s="2"/>
+      <c r="B276" s="2" t="s">
+        <v>776</v>
+      </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B277" s="2"/>
+      <c r="B277" s="2" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B278" s="2"/>
+      <c r="B278" s="2" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B279" s="2"/>
+      <c r="B279" s="2" t="s">
+        <v>779</v>
+      </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B280" s="2"/>
+      <c r="B280" s="2" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B281" s="2"/>
+      <c r="B281" s="2" t="s">
+        <v>781</v>
+      </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B282" s="2"/>
+      <c r="B282" s="2" t="s">
+        <v>782</v>
+      </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B283" s="2"/>
+      <c r="B283" s="2" t="s">
+        <v>783</v>
+      </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B284" s="2"/>
+      <c r="B284" s="2" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="285" spans="1:2">
       <c r="A285" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B285" s="2"/>
+      <c r="B285" s="2" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B286" s="2"/>
+      <c r="B286" s="2" t="s">
+        <v>786</v>
+      </c>
     </row>
     <row r="287" spans="1:2">
       <c r="A287" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B287" s="2"/>
+      <c r="B287" s="2" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B288" s="2"/>
+      <c r="B288" s="2" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B289" s="2"/>
+      <c r="B289" s="2" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="290" spans="1:2">
       <c r="A290" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B290" s="2"/>
+      <c r="B290" s="2" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="291" spans="1:2">
       <c r="A291" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B291" s="2"/>
+      <c r="B291" s="2" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="292" spans="1:2">
       <c r="A292" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B292" s="2"/>
+      <c r="B292" s="2" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="293" spans="1:2">
       <c r="A293" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B293" s="2"/>
+      <c r="B293" s="2" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="294" spans="1:2">
       <c r="A294" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B294" s="2"/>
+      <c r="B294" s="2" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="295" spans="1:2">
       <c r="A295" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B295" s="2"/>
+      <c r="B295" s="2" t="s">
+        <v>795</v>
+      </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B296" s="2"/>
+      <c r="B296" s="2" t="s">
+        <v>796</v>
+      </c>
     </row>
     <row r="297" spans="1:2">
       <c r="A297" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B297" s="2"/>
+      <c r="B297" s="2" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B298" s="2"/>
+      <c r="B298" s="2" t="s">
+        <v>798</v>
+      </c>
     </row>
     <row r="299" spans="1:2">
       <c r="A299" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B299" s="2"/>
+      <c r="B299" s="2" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="300" spans="1:2">
       <c r="A300" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B300" s="2"/>
+      <c r="B300" s="2" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="301" spans="1:2">
       <c r="A301" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B301" s="2"/>
+      <c r="B301" s="2" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="302" spans="1:2">
       <c r="A302" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B302" s="2"/>
+      <c r="B302" s="2" t="s">
+        <v>802</v>
+      </c>
     </row>
     <row r="303" spans="1:2">
       <c r="A303" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B303" s="2"/>
+      <c r="B303" s="2" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="304" spans="1:2">
       <c r="A304" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B304" s="2"/>
+      <c r="B304" s="2" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="305" spans="1:2">
       <c r="A305" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B305" s="2"/>
+      <c r="B305" s="2" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="306" spans="1:2">
       <c r="A306" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B306" s="2"/>
+      <c r="B306" s="2" t="s">
+        <v>806</v>
+      </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B307" s="2"/>
+      <c r="B307" s="2" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="308" spans="1:2">
       <c r="A308" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B308" s="2"/>
+      <c r="B308" s="2" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="309" spans="1:2">
       <c r="A309" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B309" s="2"/>
+      <c r="B309" s="2" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="310" spans="1:2">
       <c r="A310" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B310" s="2"/>
+      <c r="B310" s="2" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="311" spans="1:2">
       <c r="A311" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B311" s="2"/>
+      <c r="B311" s="2" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B312" s="2"/>
+      <c r="B312" s="2" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="313" spans="1:2">
       <c r="A313" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B313" s="2"/>
+      <c r="B313" s="2" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="314" spans="1:2">
       <c r="A314" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B314" s="2"/>
+      <c r="B314" s="2" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="315" spans="1:2">
       <c r="A315" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B315" s="2"/>
+      <c r="B315" s="2" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="316" spans="1:2">
       <c r="A316" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B316" s="2"/>
+      <c r="B316" s="2" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="317" spans="1:2">
       <c r="A317" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B317" s="2"/>
+      <c r="B317" s="2" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="318" spans="1:2">
       <c r="A318" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B318" s="2"/>
+      <c r="B318" s="2" t="s">
+        <v>818</v>
+      </c>
     </row>
     <row r="319" spans="1:2">
       <c r="A319" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B319" s="2"/>
+      <c r="B319" s="2" t="s">
+        <v>819</v>
+      </c>
     </row>
     <row r="320" spans="1:2">
       <c r="A320" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B320" s="2"/>
+      <c r="B320" s="2" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="321" spans="1:2">
       <c r="A321" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B321" s="2"/>
+      <c r="B321" s="2" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="322" spans="1:2">
       <c r="A322" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B322" s="2"/>
+      <c r="B322" s="2" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="323" spans="1:2">
       <c r="A323" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B323" s="2"/>
+      <c r="B323" s="2" t="s">
+        <v>823</v>
+      </c>
     </row>
     <row r="324" spans="1:2">
       <c r="A324" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B324" s="2"/>
+      <c r="B324" s="2" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="325" spans="1:2">
       <c r="A325" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B325" s="2"/>
+      <c r="B325" s="2" t="s">
+        <v>825</v>
+      </c>
     </row>
     <row r="326" spans="1:2">
       <c r="A326" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B326" s="2"/>
+      <c r="B326" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="327" spans="1:2">
       <c r="A327" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B327" s="2"/>
+      <c r="B327" s="2" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="328" spans="1:2">
       <c r="A328" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B328" s="2"/>
+      <c r="B328" s="2" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="329" spans="1:2">
       <c r="A329" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B329" s="2"/>
+      <c r="B329" s="2" t="s">
+        <v>829</v>
+      </c>
     </row>
     <row r="330" spans="1:2">
       <c r="A330" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B330" s="2"/>
+      <c r="B330" s="2" t="s">
+        <v>830</v>
+      </c>
     </row>
     <row r="331" spans="1:2">
       <c r="A331" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B331" s="2"/>
+      <c r="B331" s="2" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="332" spans="1:2">
       <c r="A332" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B332" s="2"/>
+      <c r="B332" s="2" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="333" spans="1:2">
       <c r="A333" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B333" s="2"/>
+      <c r="B333" s="2" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="334" spans="1:2">
       <c r="A334" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B334" s="2"/>
+      <c r="B334" s="2" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="335" spans="1:2">
       <c r="A335" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B335" s="2"/>
+      <c r="B335" s="2" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="336" spans="1:2">
       <c r="A336" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B336" s="2"/>
+      <c r="B336" s="2" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="337" spans="1:2">
       <c r="A337" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B337" s="2"/>
+      <c r="B337" s="2" t="s">
+        <v>837</v>
+      </c>
     </row>
     <row r="338" spans="1:2">
       <c r="A338" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B338" s="2"/>
+      <c r="B338" s="2" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="339" spans="1:2">
       <c r="A339" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B339" s="2"/>
+      <c r="B339" s="2" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="340" spans="1:2">
       <c r="A340" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B340" s="2"/>
+      <c r="B340" s="2" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="341" spans="1:2">
       <c r="A341" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B341" s="2"/>
+      <c r="B341" s="2" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="342" spans="1:2">
       <c r="A342" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B342" s="2"/>
+      <c r="B342" s="2" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="343" spans="1:2">
       <c r="A343" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B343" s="2"/>
+      <c r="B343" s="2" t="s">
+        <v>843</v>
+      </c>
     </row>
     <row r="344" spans="1:2">
       <c r="A344" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B344" s="2"/>
+      <c r="B344" s="2" t="s">
+        <v>844</v>
+      </c>
     </row>
     <row r="345" spans="1:2">
       <c r="A345" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B345" s="2"/>
+      <c r="B345" s="2" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="346" spans="1:2">
       <c r="A346" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B346" s="2"/>
+      <c r="B346" s="2" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="347" spans="1:2">
       <c r="A347" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B347" s="2"/>
+      <c r="B347" s="2" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="348" spans="1:2">
       <c r="A348" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B348" s="2"/>
+      <c r="B348" s="2" t="s">
+        <v>848</v>
+      </c>
     </row>
     <row r="349" spans="1:2">
       <c r="A349" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B349" s="2"/>
+      <c r="B349" s="2" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="350" spans="1:2">
       <c r="A350" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B350" s="2"/>
+      <c r="B350" s="2" t="s">
+        <v>850</v>
+      </c>
     </row>
     <row r="351" spans="1:2">
       <c r="A351" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B351" s="2"/>
+      <c r="B351" s="2" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="352" spans="1:2">
       <c r="A352" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B352" s="2"/>
+      <c r="B352" s="2" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="353" spans="1:2">
       <c r="A353" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B353" s="2"/>
+      <c r="B353" s="2" t="s">
+        <v>853</v>
+      </c>
     </row>
     <row r="354" spans="1:2">
       <c r="A354" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B354" s="2"/>
+      <c r="B354" s="2" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="355" spans="1:2">
       <c r="A355" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B355" s="2"/>
+      <c r="B355" s="2" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="356" spans="1:2">
       <c r="A356" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B356" s="2"/>
+      <c r="B356" s="2" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="357" spans="1:2">
       <c r="A357" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B357" s="2"/>
+      <c r="B357" s="2" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="358" spans="1:2">
       <c r="A358" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B358" s="2"/>
+      <c r="B358" s="2" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="359" spans="1:2">
       <c r="A359" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B359" s="2"/>
+      <c r="B359" s="2" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="360" spans="1:2">
       <c r="A360" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B360" s="2"/>
+      <c r="B360" s="2" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="361" spans="1:2">
       <c r="A361" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B361" s="2"/>
+      <c r="B361" s="2" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="362" spans="1:2">
       <c r="A362" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B362" s="2"/>
+      <c r="B362" s="2" t="s">
+        <v>862</v>
+      </c>
     </row>
     <row r="363" spans="1:2">
       <c r="A363" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B363" s="2"/>
+      <c r="B363" s="2" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="364" spans="1:2">
       <c r="A364" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B364" s="2"/>
+      <c r="B364" s="2" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="365" spans="1:2">
       <c r="A365" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B365" s="2"/>
+      <c r="B365" s="2" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="366" spans="1:2">
       <c r="A366" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B366" s="2"/>
+      <c r="B366" s="2" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="367" spans="1:2">
       <c r="A367" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B367" s="2"/>
+      <c r="B367" s="2" t="s">
+        <v>867</v>
+      </c>
     </row>
     <row r="368" spans="1:2">
       <c r="A368" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B368" s="2"/>
+      <c r="B368" s="2" t="s">
+        <v>868</v>
+      </c>
     </row>
     <row r="369" spans="1:2">
       <c r="A369" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B369" s="2"/>
+      <c r="B369" s="2" t="s">
+        <v>869</v>
+      </c>
     </row>
     <row r="370" spans="1:2">
       <c r="A370" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B370" s="2"/>
+      <c r="B370" s="2" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="371" spans="1:2">
       <c r="A371" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B371" s="2"/>
+      <c r="B371" s="2" t="s">
+        <v>871</v>
+      </c>
     </row>
     <row r="372" spans="1:2">
       <c r="A372" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B372" s="2"/>
+      <c r="B372" s="2" t="s">
+        <v>872</v>
+      </c>
     </row>
     <row r="373" spans="1:2">
       <c r="A373" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B373" s="2"/>
+      <c r="B373" s="2" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="374" spans="1:2">
       <c r="A374" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B374" s="2"/>
+      <c r="B374" s="2" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="375" spans="1:2">
       <c r="A375" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B375" s="2"/>
+      <c r="B375" s="2" t="s">
+        <v>875</v>
+      </c>
     </row>
     <row r="376" spans="1:2">
       <c r="A376" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B376" s="2"/>
+      <c r="B376" s="2" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="377" spans="1:2">
       <c r="A377" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B377" s="2"/>
+      <c r="B377" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="378" spans="1:2">
       <c r="A378" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B378" s="2"/>
+      <c r="B378" s="2" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="379" spans="1:2">
       <c r="A379" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B379" s="2"/>
+      <c r="B379" s="2" t="s">
+        <v>879</v>
+      </c>
     </row>
     <row r="380" spans="1:2">
       <c r="A380" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B380" s="2"/>
+      <c r="B380" s="2" t="s">
+        <v>880</v>
+      </c>
     </row>
     <row r="381" spans="1:2">
       <c r="A381" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B381" s="2"/>
+      <c r="B381" s="2" t="s">
+        <v>881</v>
+      </c>
     </row>
     <row r="382" spans="1:2">
       <c r="A382" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B382" s="2"/>
+      <c r="B382" s="2" t="s">
+        <v>882</v>
+      </c>
     </row>
     <row r="383" spans="1:2">
       <c r="A383" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B383" s="2"/>
+      <c r="B383" s="2" t="s">
+        <v>883</v>
+      </c>
     </row>
     <row r="384" spans="1:2">
       <c r="A384" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B384" s="2"/>
+      <c r="B384" s="2" t="s">
+        <v>884</v>
+      </c>
     </row>
     <row r="385" spans="1:2">
       <c r="A385" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B385" s="2"/>
+      <c r="B385" s="2" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="386" spans="1:2">
       <c r="A386" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B386" s="2"/>
+      <c r="B386" s="2" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="387" spans="1:2">
       <c r="A387" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B387" s="2"/>
+      <c r="B387" s="2" t="s">
+        <v>887</v>
+      </c>
     </row>
     <row r="388" spans="1:2">
       <c r="A388" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B388" s="2"/>
+      <c r="B388" s="2" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="389" spans="1:2">
       <c r="A389" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B389" s="2"/>
+      <c r="B389" s="2" t="s">
+        <v>889</v>
+      </c>
     </row>
     <row r="390" spans="1:2">
       <c r="A390" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B390" s="2"/>
+      <c r="B390" s="2" t="s">
+        <v>890</v>
+      </c>
     </row>
     <row r="391" spans="1:2">
       <c r="A391" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B391" s="2"/>
+      <c r="B391" s="2" t="s">
+        <v>891</v>
+      </c>
     </row>
     <row r="392" spans="1:2">
       <c r="A392" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B392" s="2"/>
+      <c r="B392" s="2" t="s">
+        <v>892</v>
+      </c>
     </row>
     <row r="393" spans="1:2">
       <c r="A393" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B393" s="2"/>
+      <c r="B393" s="2" t="s">
+        <v>893</v>
+      </c>
     </row>
     <row r="394" spans="1:2">
       <c r="A394" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B394" s="2"/>
+      <c r="B394" s="2" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="395" spans="1:2">
       <c r="A395" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B395" s="2"/>
+      <c r="B395" s="2" t="s">
+        <v>895</v>
+      </c>
     </row>
     <row r="396" spans="1:2">
       <c r="A396" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="B396" s="2"/>
+      <c r="B396" s="2" t="s">
+        <v>896</v>
+      </c>
     </row>
     <row r="397" spans="1:2">
       <c r="A397" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B397" s="2"/>
+      <c r="B397" s="2" t="s">
+        <v>897</v>
+      </c>
     </row>
     <row r="398" spans="1:2">
       <c r="A398" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B398" s="2"/>
+      <c r="B398" s="2" t="s">
+        <v>898</v>
+      </c>
     </row>
     <row r="399" spans="1:2">
       <c r="A399" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B399" s="2"/>
+      <c r="B399" s="2" t="s">
+        <v>899</v>
+      </c>
     </row>
     <row r="400" spans="1:2">
       <c r="A400" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="B400" s="2"/>
+      <c r="B400" s="2" t="s">
+        <v>900</v>
+      </c>
     </row>
     <row r="401" spans="1:2">
       <c r="A401" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B401" s="2"/>
+      <c r="B401" s="2" t="s">
+        <v>901</v>
+      </c>
     </row>
     <row r="402" spans="1:2">
       <c r="A402" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="B402" s="2"/>
+      <c r="B402" s="2" t="s">
+        <v>902</v>
+      </c>
     </row>
     <row r="403" spans="1:2">
       <c r="A403" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="B403" s="2"/>
+      <c r="B403" s="2" t="s">
+        <v>903</v>
+      </c>
     </row>
     <row r="404" spans="1:2">
       <c r="A404" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B404" s="2"/>
+      <c r="B404" s="2" t="s">
+        <v>904</v>
+      </c>
     </row>
     <row r="405" spans="1:2">
       <c r="A405" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="B405" s="2"/>
+      <c r="B405" s="2" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="406" spans="1:2">
       <c r="A406" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="B406" s="2"/>
+      <c r="B406" s="2" t="s">
+        <v>906</v>
+      </c>
     </row>
     <row r="407" spans="1:2">
       <c r="A407" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B407" s="2"/>
+      <c r="B407" s="2" t="s">
+        <v>907</v>
+      </c>
     </row>
     <row r="408" spans="1:2">
       <c r="A408" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="B408" s="2"/>
+      <c r="B408" s="2" t="s">
+        <v>908</v>
+      </c>
     </row>
     <row r="409" spans="1:2">
       <c r="A409" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="B409" s="2"/>
+      <c r="B409" s="2" t="s">
+        <v>909</v>
+      </c>
     </row>
     <row r="410" spans="1:2">
       <c r="A410" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B410" s="2"/>
+      <c r="B410" s="2" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="411" spans="1:2">
       <c r="A411" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="B411" s="2"/>
+      <c r="B411" s="2" t="s">
+        <v>911</v>
+      </c>
     </row>
     <row r="412" spans="1:2">
       <c r="A412" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B412" s="2"/>
+      <c r="B412" s="2" t="s">
+        <v>912</v>
+      </c>
     </row>
     <row r="413" spans="1:2">
       <c r="A413" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B413" s="2"/>
+      <c r="B413" s="2" t="s">
+        <v>913</v>
+      </c>
     </row>
     <row r="414" spans="1:2">
       <c r="A414" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B414" s="2"/>
+      <c r="B414" s="2" t="s">
+        <v>914</v>
+      </c>
     </row>
     <row r="415" spans="1:2">
       <c r="A415" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B415" s="2"/>
+      <c r="B415" s="2" t="s">
+        <v>915</v>
+      </c>
     </row>
     <row r="416" spans="1:2">
       <c r="A416" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B416" s="2"/>
+      <c r="B416" s="2" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="417" spans="1:2">
       <c r="A417" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="B417" s="2"/>
+      <c r="B417" s="2" t="s">
+        <v>917</v>
+      </c>
     </row>
     <row r="418" spans="1:2">
       <c r="A418" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="B418" s="2"/>
+      <c r="B418" s="2" t="s">
+        <v>918</v>
+      </c>
     </row>
     <row r="419" spans="1:2">
       <c r="A419" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B419" s="2"/>
+      <c r="B419" s="2" t="s">
+        <v>919</v>
+      </c>
     </row>
     <row r="420" spans="1:2">
       <c r="A420" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B420" s="2"/>
+      <c r="B420" s="2" t="s">
+        <v>920</v>
+      </c>
     </row>
     <row r="421" spans="1:2">
       <c r="A421" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="B421" s="2"/>
+      <c r="B421" s="2" t="s">
+        <v>921</v>
+      </c>
     </row>
     <row r="422" spans="1:2">
       <c r="A422" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="B422" s="2"/>
+      <c r="B422" s="2" t="s">
+        <v>922</v>
+      </c>
     </row>
     <row r="423" spans="1:2">
       <c r="A423" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B423" s="2"/>
+      <c r="B423" s="2" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="424" spans="1:2">
       <c r="A424" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="B424" s="2"/>
+      <c r="B424" s="2" t="s">
+        <v>924</v>
+      </c>
     </row>
     <row r="425" spans="1:2">
       <c r="A425" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="B425" s="2"/>
+      <c r="B425" s="2" t="s">
+        <v>925</v>
+      </c>
     </row>
     <row r="426" spans="1:2">
       <c r="A426" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="B426" s="2"/>
+      <c r="B426" s="2" t="s">
+        <v>926</v>
+      </c>
     </row>
     <row r="427" spans="1:2">
       <c r="A427" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B427" s="2"/>
+      <c r="B427" s="2" t="s">
+        <v>927</v>
+      </c>
     </row>
     <row r="428" spans="1:2">
       <c r="A428" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B428" s="2"/>
+      <c r="B428" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
     <row r="429" spans="1:2">
       <c r="A429" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="B429" s="2"/>
+      <c r="B429" s="2" t="s">
+        <v>929</v>
+      </c>
     </row>
     <row r="430" spans="1:2">
       <c r="A430" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B430" s="2"/>
+      <c r="B430" s="2" t="s">
+        <v>930</v>
+      </c>
     </row>
     <row r="431" spans="1:2">
       <c r="A431" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="B431" s="2"/>
+      <c r="B431" s="2" t="s">
+        <v>931</v>
+      </c>
     </row>
     <row r="432" spans="1:2">
       <c r="A432" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B432" s="2"/>
+      <c r="B432" s="2" t="s">
+        <v>932</v>
+      </c>
     </row>
     <row r="433" spans="1:2">
       <c r="A433" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B433" s="2"/>
+      <c r="B433" s="2" t="s">
+        <v>933</v>
+      </c>
     </row>
     <row r="434" spans="1:2">
       <c r="A434" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="B434" s="2"/>
+      <c r="B434" s="2" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="435" spans="1:2">
       <c r="A435" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B435" s="2"/>
+      <c r="B435" s="2" t="s">
+        <v>935</v>
+      </c>
     </row>
     <row r="436" spans="1:2">
       <c r="A436" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B436" s="2"/>
+      <c r="B436" s="2" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="437" spans="1:2">
       <c r="A437" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B437" s="2"/>
+      <c r="B437" s="2" t="s">
+        <v>937</v>
+      </c>
     </row>
     <row r="438" spans="1:2">
       <c r="A438" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="B438" s="2"/>
+      <c r="B438" s="2" t="s">
+        <v>938</v>
+      </c>
     </row>
     <row r="439" spans="1:2">
       <c r="A439" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="B439" s="2"/>
+      <c r="B439" s="2" t="s">
+        <v>939</v>
+      </c>
     </row>
     <row r="440" spans="1:2">
       <c r="A440" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="B440" s="2"/>
+      <c r="B440" s="2" t="s">
+        <v>940</v>
+      </c>
     </row>
     <row r="441" spans="1:2">
       <c r="A441" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="B441" s="2"/>
+      <c r="B441" s="2" t="s">
+        <v>941</v>
+      </c>
     </row>
     <row r="442" spans="1:2">
       <c r="A442" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="B442" s="2"/>
+      <c r="B442" s="2" t="s">
+        <v>942</v>
+      </c>
     </row>
     <row r="443" spans="1:2">
       <c r="A443" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="B443" s="2"/>
+      <c r="B443" s="2" t="s">
+        <v>943</v>
+      </c>
     </row>
     <row r="444" spans="1:2">
       <c r="A444" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="B444" s="2"/>
+      <c r="B444" s="2" t="s">
+        <v>944</v>
+      </c>
     </row>
     <row r="445" spans="1:2">
       <c r="A445" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B445" s="2"/>
+      <c r="B445" s="2" t="s">
+        <v>945</v>
+      </c>
     </row>
     <row r="446" spans="1:2">
       <c r="A446" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="B446" s="2"/>
+      <c r="B446" s="2" t="s">
+        <v>946</v>
+      </c>
     </row>
     <row r="447" spans="1:2">
       <c r="A447" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="B447" s="2"/>
+      <c r="B447" s="2" t="s">
+        <v>947</v>
+      </c>
     </row>
     <row r="448" spans="1:2">
       <c r="A448" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="B448" s="2"/>
+      <c r="B448" s="2" t="s">
+        <v>948</v>
+      </c>
     </row>
     <row r="449" spans="1:2">
       <c r="A449" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="B449" s="2"/>
+      <c r="B449" s="2" t="s">
+        <v>949</v>
+      </c>
     </row>
     <row r="450" spans="1:2">
       <c r="A450" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B450" s="2"/>
+      <c r="B450" s="2" t="s">
+        <v>950</v>
+      </c>
     </row>
     <row r="451" spans="1:2">
       <c r="A451" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="B451" s="2"/>
+      <c r="B451" s="2" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="452" spans="1:2">
       <c r="A452" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="B452" s="2"/>
+      <c r="B452" s="2" t="s">
+        <v>952</v>
+      </c>
     </row>
     <row r="453" spans="1:2">
       <c r="A453" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="B453" s="2"/>
+      <c r="B453" s="2" t="s">
+        <v>953</v>
+      </c>
     </row>
     <row r="454" spans="1:2">
       <c r="A454" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B454" s="2"/>
+      <c r="B454" s="2" t="s">
+        <v>954</v>
+      </c>
     </row>
     <row r="455" spans="1:2">
       <c r="A455" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="B455" s="2"/>
+      <c r="B455" s="2" t="s">
+        <v>955</v>
+      </c>
     </row>
     <row r="456" spans="1:2">
       <c r="A456" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B456" s="2"/>
+      <c r="B456" s="2" t="s">
+        <v>956</v>
+      </c>
     </row>
     <row r="457" spans="1:2">
       <c r="A457" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="B457" s="2"/>
+      <c r="B457" s="2" t="s">
+        <v>957</v>
+      </c>
     </row>
     <row r="458" spans="1:2">
       <c r="A458" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="B458" s="2"/>
+      <c r="B458" s="2" t="s">
+        <v>958</v>
+      </c>
     </row>
     <row r="459" spans="1:2">
       <c r="A459" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="B459" s="2"/>
+      <c r="B459" s="2" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="460" spans="1:2">
       <c r="A460" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="B460" s="2"/>
+      <c r="B460" s="2" t="s">
+        <v>960</v>
+      </c>
     </row>
     <row r="461" spans="1:2">
       <c r="A461" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B461" s="2"/>
+      <c r="B461" s="2" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="462" spans="1:2">
       <c r="A462" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="B462" s="2"/>
+      <c r="B462" s="2" t="s">
+        <v>962</v>
+      </c>
     </row>
     <row r="463" spans="1:2">
       <c r="A463" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="B463" s="2"/>
+      <c r="B463" s="2" t="s">
+        <v>963</v>
+      </c>
     </row>
     <row r="464" spans="1:2">
       <c r="A464" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="B464" s="2"/>
+      <c r="B464" s="2" t="s">
+        <v>964</v>
+      </c>
     </row>
     <row r="465" spans="1:2">
       <c r="A465" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B465" s="2"/>
+      <c r="B465" s="2" t="s">
+        <v>965</v>
+      </c>
     </row>
     <row r="466" spans="1:2">
       <c r="A466" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="B466" s="2"/>
+      <c r="B466" s="2" t="s">
+        <v>966</v>
+      </c>
     </row>
     <row r="467" spans="1:2">
       <c r="A467" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="B467" s="2"/>
+      <c r="B467" s="2" t="s">
+        <v>967</v>
+      </c>
     </row>
     <row r="468" spans="1:2">
       <c r="A468" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="B468" s="2"/>
+      <c r="B468" s="2" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="469" spans="1:2">
       <c r="A469" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="B469" s="2"/>
+      <c r="B469" s="2" t="s">
+        <v>969</v>
+      </c>
     </row>
     <row r="470" spans="1:2">
       <c r="A470" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="B470" s="2"/>
+      <c r="B470" s="2" t="s">
+        <v>970</v>
+      </c>
     </row>
     <row r="471" spans="1:2">
       <c r="A471" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="B471" s="2"/>
+      <c r="B471" s="2" t="s">
+        <v>971</v>
+      </c>
     </row>
     <row r="472" spans="1:2">
       <c r="A472" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B472" s="2"/>
+      <c r="B472" s="2" t="s">
+        <v>972</v>
+      </c>
     </row>
     <row r="473" spans="1:2">
       <c r="A473" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="B473" s="2"/>
+      <c r="B473" s="2" t="s">
+        <v>973</v>
+      </c>
     </row>
     <row r="474" spans="1:2">
       <c r="A474" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="B474" s="2"/>
+      <c r="B474" s="2" t="s">
+        <v>974</v>
+      </c>
     </row>
     <row r="475" spans="1:2">
       <c r="A475" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="B475" s="2"/>
+      <c r="B475" s="2" t="s">
+        <v>975</v>
+      </c>
     </row>
     <row r="476" spans="1:2">
       <c r="A476" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="B476" s="2"/>
+      <c r="B476" s="2" t="s">
+        <v>976</v>
+      </c>
     </row>
     <row r="477" spans="1:2">
       <c r="A477" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="B477" s="2"/>
+      <c r="B477" s="2" t="s">
+        <v>977</v>
+      </c>
     </row>
     <row r="478" spans="1:2">
       <c r="A478" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="B478" s="2"/>
+      <c r="B478" s="2" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="479" spans="1:2">
       <c r="A479" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="B479" s="2"/>
+      <c r="B479" s="2" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="480" spans="1:2">
       <c r="A480" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="B480" s="2"/>
+      <c r="B480" s="2" t="s">
+        <v>980</v>
+      </c>
     </row>
     <row r="481" spans="1:2">
       <c r="A481" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="B481" s="2"/>
+      <c r="B481" s="2" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="482" spans="1:2">
       <c r="A482" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B482" s="2"/>
+      <c r="B482" s="2" t="s">
+        <v>982</v>
+      </c>
     </row>
     <row r="483" spans="1:2">
       <c r="A483" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="B483" s="2"/>
+      <c r="B483" s="2" t="s">
+        <v>983</v>
+      </c>
     </row>
     <row r="484" spans="1:2">
       <c r="A484" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B484" s="2"/>
+      <c r="B484" s="2" t="s">
+        <v>984</v>
+      </c>
     </row>
     <row r="485" spans="1:2">
       <c r="A485" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="B485" s="2"/>
+      <c r="B485" s="2" t="s">
+        <v>985</v>
+      </c>
     </row>
     <row r="486" spans="1:2">
       <c r="A486" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="B486" s="2"/>
+      <c r="B486" s="2" t="s">
+        <v>986</v>
+      </c>
     </row>
     <row r="487" spans="1:2">
       <c r="A487" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="B487" s="2"/>
+      <c r="B487" s="2" t="s">
+        <v>987</v>
+      </c>
     </row>
     <row r="488" spans="1:2">
       <c r="A488" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="B488" s="2"/>
+      <c r="B488" s="2" t="s">
+        <v>988</v>
+      </c>
     </row>
     <row r="489" spans="1:2">
       <c r="A489" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="B489" s="2"/>
+      <c r="B489" s="2" t="s">
+        <v>989</v>
+      </c>
     </row>
     <row r="490" spans="1:2">
       <c r="A490" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="B490" s="2"/>
+      <c r="B490" s="2" t="s">
+        <v>990</v>
+      </c>
     </row>
     <row r="491" spans="1:2">
       <c r="A491" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="B491" s="2"/>
+      <c r="B491" s="2" t="s">
+        <v>991</v>
+      </c>
     </row>
     <row r="492" spans="1:2">
       <c r="A492" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="B492" s="2"/>
+      <c r="B492" s="2" t="s">
+        <v>992</v>
+      </c>
     </row>
     <row r="493" spans="1:2">
       <c r="A493" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="B493" s="2"/>
+      <c r="B493" s="2" t="s">
+        <v>993</v>
+      </c>
     </row>
     <row r="494" spans="1:2">
       <c r="A494" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="B494" s="2"/>
+      <c r="B494" s="2" t="s">
+        <v>994</v>
+      </c>
     </row>
     <row r="495" spans="1:2">
       <c r="A495" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="B495" s="2"/>
+      <c r="B495" s="2" t="s">
+        <v>995</v>
+      </c>
     </row>
     <row r="496" spans="1:2">
       <c r="A496" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B496" s="2"/>
+      <c r="B496" s="2" t="s">
+        <v>996</v>
+      </c>
     </row>
     <row r="497" spans="1:2">
       <c r="A497" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="B497" s="2"/>
+      <c r="B497" s="2" t="s">
+        <v>997</v>
+      </c>
     </row>
     <row r="498" spans="1:2">
       <c r="A498" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="B498" s="2"/>
+      <c r="B498" s="2" t="s">
+        <v>998</v>
+      </c>
     </row>
     <row r="499" spans="1:2">
       <c r="A499" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="B499" s="2"/>
+      <c r="B499" s="2" t="s">
+        <v>999</v>
+      </c>
     </row>
     <row r="500" spans="1:2">
       <c r="A500" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="B500" s="2"/>
+      <c r="B500" s="2" t="s">
+        <v>1000</v>
+      </c>
     </row>
     <row r="501" spans="1:2">
       <c r="A501" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="B501" s="2"/>
+      <c r="B501" s="2" t="s">
+        <v>1001</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committed on 02:03:2018:11:04:00PM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Episerver_Campaign_Validation_500.xlsx
+++ b/data/Episerver_Campaign_Validation_500.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\workspace\Ameex_Marketing_Team\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="935">
   <si>
     <t>Email ID</t>
   </si>
@@ -2076,19 +2081,1189 @@
   </si>
   <si>
     <t>gina.estrada@capmetro.org</t>
+  </si>
+  <si>
+    <t>darlene.einerson@kindredhealthcare.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>darryl.wilburn@hobartcorp.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dasnyder@sc4.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dave.smith@stvincent.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dave@harrisadvisory.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dave@opwealthmanagement.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dave@s2imaging.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>davef@nimlok.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>davefranchak@maximhealthsystems.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>davem@pegsummit.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.ashman@longbeach.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.beamer@fei.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>David.Bergstrom@couragecenter.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.coleman@amecfw.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.dibben@cso.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.hill@sgc-financial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.kanihan@allina.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.lancett@gofallon.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.lechner@lifewiseor.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.lloyd@intelliresponse.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>David.Macpherson@caprelo.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>David.Mclean@nov.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>David.McQuiggan@densitron.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.millican@xerox.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.milmore@libertymedical.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.resnick@clarke.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david.smallwood@bangor.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@air1.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@beauchampbenefits.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@harrisadvisory.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@highlandmoneymgmt.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@jacobgold.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@klove.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@maynardwealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>David@mcleanwealthpartners.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@monecoadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@ralickicpa.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@richmondandassociatesllc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if david@sentinelrockwm.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@tomasettigroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david@weinerinsurance.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david_curchy@cbolobank.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>davidb@bendixfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if davidbruzzese@mercydurango.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>davidd@aileronwm.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>davison@sfcinc.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dawn.anderson@amnhealthcare.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dawn.nylander@trgc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dawn.safford@carestream.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dawn@bbcommercialsolutions.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dawn@mannorfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dawnevola@lakeviewfc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dbach@wycokck.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dbaden@secantcorp.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dbarnes@nctm.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dberg@waukeshacounty.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dbibby@nmhc.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>DBillerbeck@siimage.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dblansfield@ntmllc.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dbollman@acep.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dbooth@bfa1.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dborofsky@hodges.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dbrady@onehoustonfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dbrooks@carnegiehall.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dcaiazzo@playmeadowlands.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dcampagna@fmhc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dcarozza@acfe.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dcarr@spunkmeyer.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dcb@lbwl.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dcervantes@uso.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dchandler@martinfinancialgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dchapman@alliedwealthpartners.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dchase@bolingbrookparks.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dchin@arvo.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dclabo@cityofpigeonforge.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dclark@theheartcenter.net
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dcollege@dean.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dcordeiro@techinsights.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if DCoriale@Delcor.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dcostello@pfmadvisor.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ddaugherty@preservewealthok.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dderousie@williamcharleswest.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ddesiderio@rer.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ddonahue@ncpga.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ddraper@SapphireBlueIP.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dduran@southeastmn.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ddurr@romehospital.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>deanne.raymond@laitram.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if deannkarlson@diiketchikan.net
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>deb.rizzi@unitedwater.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>debbi@jdbowenfinancialgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>debbie@anytown.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>deborah@dallascan.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>deborah@mattjelnickycfp.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dechelberger@anchoraccounting.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dedwards@sheltergrp.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dek@lavezzi.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>demerson@virginia.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>denise.green@pinnadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dennis.rush@windstream.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dennis.schleper@claconnect.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dennis@jdhadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Dennis@swfinancialgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Dennis@wealthadvisorsoffice.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>derekrichards@sailingrowing.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>derrick.toigo@infrastructureontario.ca is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dertel@vantagepartners.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dervla.kelly@corusent.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>devin.milton@astro.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dfiorenza@sgretirementplanners.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dflaim@selectmedical.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dgasparovic@garaga.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dgaston@douglascountybank.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dgiglio@naceweb.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dgrooms@iapropane.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dhermann@ziegler.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dhill@vidanthealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dhouchins@onehoustonfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dhovland@saberdentalstudio.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>diana.wallis@coloradohealth.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>diane.laurent@milliman.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dick@fpgkc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dick@martinfinancialgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dick@mvpdesign.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dickens@lindehc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>diegog@sdhc.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dillen@mrs.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dino@mbwmg.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>disdahl@loram.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>djb@bartolfwealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>djoanis@telamon.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>djohnson@octa.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if djohnston@idsociety.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>DJones@pequotmuseum.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dkempton@franciscan.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dkenyon@jewelersboard.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dklim@aptanj.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dkreeger@certapro.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dlindholm@cost.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dlouthain@alacep.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dluber@armorwealthgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dlundquist@romehospital.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if DLynch@miriamhospital.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dm@marshallwealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dmartin@juhlbrokerage.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dmcrbide@mcbridefinancial.net is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dmedley@theabfm.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dmello@knowledgefoundation.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dmoore@acosta.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dobbinsj@chiefautomotive.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Don.Pawelko@spscientific.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>don@baysidefinancialgroup.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>don@nimlok-kentucky.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>don_erlanger@cashmanequipment.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>donald.adams@clarke.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>donald.droegemueller@lpl.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if donald.forbes@mybrighthouse.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>donald.schermerhorn@remingtoncollege.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Donna.Berry@schinnerer.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>donna.martinez@nursefinders.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>donna.thomas@burnettitlein.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>donna@msawealthmanagement.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>doug.may@magellanlp.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>doug.sehres@plantoroe.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>doug@baysidefinancialgroup.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>doug@investmentservicesinc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>doug@synventive.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dougb@dhbaker.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Douglas.Arms@kellyocg.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>douglas.newman@pinnadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dougmeadows@murfeemeadows.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dougolson@triton.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dougwilliams@myinslink.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>doyle@ntea.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dpalmisano@mag.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dpangili@saintfranciscare.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dpatane@mainstreet-financialgroup.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dplesh@asha.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dpollak@vAuto.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dpower@vcornerstone.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dr_costello@yahoo.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>drdoncut@focusfinancialgroup.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if drew.collins@tottengroup.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>drew.hayden@securianma.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>drew.vrba@medtravelers.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>drodenbush@vcornerstone.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>drogers@continentallab.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>droth@operanews.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>DRust@QuartzFinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dsam@elgin.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dsauceda@riversideresort.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dschlegel@velaw.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dsimmons@simmonscapitalgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dsinger@renalmd.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dsmith@maminvest.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dstaal@kidshopeusa.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dsutro@zachys.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dtrottier@inflexxion.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dukemm@vmi.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dusan_ravnihar@veyance.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>DusonAng@einstein.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dwatson@nysba.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dwayne.olivieri@delmarva.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dykeman.steven@irvingequipment.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dzale@zalecapital.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dzanini@arda.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>e.emekauwa@wshafm.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>e_felder@culinary.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eabrock@msdperformance.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eadie.peter@jdilogistics.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if ealonsomendoza@agbell.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ebirchm@michfb.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>EBloom@sirspeedy.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ebonnell@cox.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ebowman@thebdx.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ecuevas@pilotcatholicnews.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ed.fotsch@pdr.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if ed.smith@nationaloilwell.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ed@mcdonoughcapital.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Ed@pensionmark.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>edeangelo@crefc.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>edmonton@thomsonps.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>edward_benz@dfci.harvard.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>edwards.richard@atlantictowing.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eeickman@heartlandexpress.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>efink@dupageforest.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>efoster@pyawaltman.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>efreiberg@rascorp.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>egardiner@acls.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ehurley@primr.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ejerome@monroecollege.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ejsedwick@premierhealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ek@kgadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>elack@risd.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>elaine.bliss@crossmatch.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ELB@RyzomeAdvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if elee@bostonballet.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if elindberg@williamcharles.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>elizabeth.truesdell@allinahealth.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ellen.michael@proequities.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eltoweissymy@vmi.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if Ember.Cunningham@gvltec.edu
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>emcglinchey@secantcorp.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>EmilyBenton@PremierPlanningGroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>emma.vanness@raggedmountainresort.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>emma@wipga.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>EMoore@santafeopera.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>enilson@massdental.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>epollan@ltk.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>epotts@panoramawealthstrategies.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eprince@rentonwa.gov is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric.boxma@intralox.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric.park@lpl.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric.westerby@nygard.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric@amfar.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric@jacobsencapital.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric@lewisandmonroe.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric@preferredwealthadvisors.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric@reichassetmanagement.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eric@stibawmg.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if erica.benjamin@cmaa.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>erica.ciupak@sme.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>erica.cuyugan@smgov.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>erica@kranzinsurance.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ericaphillips@hillelatuchicago.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>erich@digitalpersona.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>erick@portessaguenay.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ericw@ccwmgmt.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>EricZ@ccwmgmt.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eriley@wwnorton.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>erin.kennedy@kindredhealthcare.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>erin.mcmann@tfgroup.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ermiller@maxhealth.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if Ernest.Leonelli@colemannatural.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ernie@stibawmg.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>erover@dana.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eryden@msdperformance.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>esagmoe@kidshopeusa.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>esalinas@wfubmc.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if ESantiago@minitab.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Essie_McGuire@mcpsmd.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>estrauss@usfca.edu is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Eva.Margolis@lssmn.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>eva.robertson@protective.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Evan@SecurEstateOnline.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>evansickle@flmedical.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ewanda.kraner@abxair.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ewhiton@zoll.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>fang@CancerPreventionInstitute.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>fara.kearnes@panfs.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>farberg@carnegiemuseums.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>farzad@strykerfinancial.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>FBazgan@cambro.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>FCostigan@pspartnersolutions.com is not
+a valid deliverable e-mail box address.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2106,160 +3281,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2278,7 +3302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2287,127 +3311,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399945066682943"/>
+        <fgColor theme="5" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399945066682943"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399945066682943"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2419,96 +3335,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399945066682943"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399945066682943"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399945066682943"/>
+        <fgColor theme="4" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2531,259 +3375,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2792,66 +3394,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="9">
+    <cellStyle name="60% - Accent1 2" xfId="6"/>
+    <cellStyle name="60% - Accent2 2" xfId="7"/>
+    <cellStyle name="60% - Accent3 2" xfId="3"/>
+    <cellStyle name="60% - Accent4 2" xfId="5"/>
+    <cellStyle name="60% - Accent5 2" xfId="1"/>
+    <cellStyle name="60% - Accent6 2" xfId="2"/>
+    <cellStyle name="Neutral 2" xfId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent5 2" xfId="1"/>
-    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
-    <cellStyle name="Comma" xfId="3" builtinId="3"/>
-    <cellStyle name="Currency" xfId="4" builtinId="4"/>
-    <cellStyle name="Comma[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Currency[0]" xfId="7" builtinId="7"/>
-    <cellStyle name="Check Cell" xfId="8" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17"/>
-    <cellStyle name="Note" xfId="10" builtinId="10"/>
-    <cellStyle name="60% - Accent6 2" xfId="11"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="13" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="15" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="16" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="17" builtinId="35"/>
-    <cellStyle name="Title" xfId="18" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="19" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="20" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="21" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="22" builtinId="19"/>
-    <cellStyle name="Input" xfId="23" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="24" builtinId="40"/>
-    <cellStyle name="Good" xfId="25" builtinId="26"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="27" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="28" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="29" builtinId="24"/>
-    <cellStyle name="Total" xfId="30" builtinId="25"/>
-    <cellStyle name="60% - Accent3 2" xfId="31"/>
-    <cellStyle name="Bad" xfId="32" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="33" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="36" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="37" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="38" builtinId="34"/>
-    <cellStyle name="Title 2" xfId="39"/>
-    <cellStyle name="20% - Accent6" xfId="40" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="41" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="42" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="43" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="44" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="45" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="46" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="47" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="48" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="49" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="50" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="51" builtinId="51"/>
-    <cellStyle name="60% - Accent4 2" xfId="52"/>
-    <cellStyle name="60% - Accent6" xfId="53" builtinId="52"/>
-    <cellStyle name="60% - Accent1 2" xfId="54"/>
-    <cellStyle name="60% - Accent2 2" xfId="55"/>
-    <cellStyle name="Neutral 2" xfId="56"/>
+    <cellStyle name="Title 2" xfId="4"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3112,18 +3675,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A427" workbookViewId="0">
+      <selection activeCell="A435" sqref="A435"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="109.714285714286" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4256,1765 +4818,2353 @@
       <c r="A142" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B142" s="2"/>
+      <c r="B142" s="2" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B143" s="2"/>
+      <c r="B143" s="2" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B144" s="2"/>
+      <c r="B144" s="2" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B145" s="2"/>
+      <c r="B145" s="2" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B146" s="2"/>
+      <c r="B146" s="2" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B147" s="2"/>
+      <c r="B147" s="2" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B148" s="2"/>
+      <c r="B148" s="2" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B149" s="2"/>
+      <c r="B149" s="2" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B150" s="2"/>
+      <c r="B150" s="2" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B151" s="2"/>
+      <c r="B151" s="2" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B152" s="2"/>
+      <c r="B152" s="2" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B153" s="2"/>
+      <c r="B153" s="2" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B154" s="2"/>
+      <c r="B154" s="2" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B155" s="2"/>
+      <c r="B155" s="2" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B156" s="2"/>
+      <c r="B156" s="2" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B157" s="2"/>
+      <c r="B157" s="2" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B158" s="2"/>
+      <c r="B158" s="2" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B159" s="2"/>
+      <c r="B159" s="2" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B160" s="2"/>
+      <c r="B160" s="2" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B161" s="2"/>
+      <c r="B161" s="2" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B162" s="2"/>
+      <c r="B162" s="2" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B163" s="2"/>
+      <c r="B163" s="2" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B164" s="2"/>
+      <c r="B164" s="2" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B165" s="2"/>
+      <c r="B165" s="2" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B166" s="2"/>
+      <c r="B166" s="2" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B167" s="2"/>
+      <c r="B167" s="2" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B168" s="2"/>
+      <c r="B168" s="2" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B169" s="2"/>
+      <c r="B169" s="2" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B170" s="2"/>
+      <c r="B170" s="2" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B171" s="2"/>
+      <c r="B171" s="2" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B172" s="2"/>
+      <c r="B172" s="2" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B173" s="2"/>
+      <c r="B173" s="2" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B174" s="2"/>
+      <c r="B174" s="2" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B175" s="2"/>
+      <c r="B175" s="2" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B176" s="2"/>
+      <c r="B176" s="2" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B177" s="2"/>
+      <c r="B177" s="2" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B178" s="2"/>
+      <c r="B178" s="2" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B179" s="2"/>
+      <c r="B179" s="2" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B180" s="2"/>
+      <c r="B180" s="2" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B181" s="2"/>
+      <c r="B181" s="2" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B182" s="2"/>
+      <c r="B182" s="2" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B183" s="2"/>
+      <c r="B183" s="2" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B184" s="2"/>
+      <c r="B184" s="2" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B185" s="2"/>
+      <c r="B185" s="2" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B186" s="2"/>
+      <c r="B186" s="2" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B187" s="2"/>
+      <c r="B187" s="2" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B188" s="2"/>
+      <c r="B188" s="2" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B189" s="2"/>
+      <c r="B189" s="2" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B190" s="2"/>
+      <c r="B190" s="2" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B191" s="2"/>
+      <c r="B191" s="2" t="s">
+        <v>690</v>
+      </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B192" s="2"/>
+      <c r="B192" s="2" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B193" s="2"/>
+      <c r="B193" s="2" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B194" s="2"/>
+      <c r="B194" s="2" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B195" s="2"/>
+      <c r="B195" s="2" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B196" s="2"/>
+      <c r="B196" s="2" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B197" s="2"/>
+      <c r="B197" s="2" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B198" s="2"/>
+      <c r="B198" s="2" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B199" s="2"/>
+      <c r="B199" s="2" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B200" s="2"/>
+      <c r="B200" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B201" s="2"/>
+      <c r="B201" s="2" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B202" s="2"/>
+      <c r="B202" s="2" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B203" s="2"/>
+      <c r="B203" s="2" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B204" s="2"/>
+      <c r="B204" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B205" s="2"/>
+      <c r="B205" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B206" s="2"/>
+      <c r="B206" s="2" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B207" s="2"/>
+      <c r="B207" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B208" s="2"/>
+      <c r="B208" s="2" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B209" s="2"/>
+      <c r="B209" s="2" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B210" s="2"/>
+      <c r="B210" s="2" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B211" s="2"/>
+      <c r="B211" s="2" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B212" s="2"/>
+      <c r="B212" s="2" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B213" s="2"/>
+      <c r="B213" s="2" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B214" s="2"/>
+      <c r="B214" s="2" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B215" s="2"/>
+      <c r="B215" s="2" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B216" s="2"/>
+      <c r="B216" s="2" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B217" s="2"/>
+      <c r="B217" s="2" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B218" s="2"/>
+      <c r="B218" s="2" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B219" s="2"/>
+      <c r="B219" s="2" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B220" s="2"/>
+      <c r="B220" s="2" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B221" s="2"/>
+      <c r="B221" s="2" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B222" s="2"/>
+      <c r="B222" s="2" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B223" s="2"/>
+      <c r="B223" s="2" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B224" s="2"/>
+      <c r="B224" s="2" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B225" s="2"/>
+      <c r="B225" s="2" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B226" s="2"/>
+      <c r="B226" s="2" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B227" s="2"/>
+      <c r="B227" s="2" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B228" s="2"/>
+      <c r="B228" s="2" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B229" s="2"/>
+      <c r="B229" s="2" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B230" s="2"/>
+      <c r="B230" s="2" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B231" s="2"/>
+      <c r="B231" s="2" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B232" s="2"/>
+      <c r="B232" s="2" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B233" s="2"/>
+      <c r="B233" s="2" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B234" s="2"/>
+      <c r="B234" s="2" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B235" s="2"/>
+      <c r="B235" s="2" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B236" s="2"/>
+      <c r="B236" s="2" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B237" s="2"/>
+      <c r="B237" s="2" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B238" s="2"/>
+      <c r="B238" s="2" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B239" s="2"/>
+      <c r="B239" s="2" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B240" s="2"/>
+      <c r="B240" s="2" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B241" s="2"/>
+      <c r="B241" s="2" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B242" s="2"/>
+      <c r="B242" s="2" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B243" s="2"/>
+      <c r="B243" s="2" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B244" s="2"/>
+      <c r="B244" s="2" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B245" s="2"/>
+      <c r="B245" s="2" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B246" s="2"/>
+      <c r="B246" s="2" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B247" s="2"/>
+      <c r="B247" s="2" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B248" s="2"/>
+      <c r="B248" s="2" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B249" s="2"/>
+      <c r="B249" s="2" t="s">
+        <v>748</v>
+      </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B250" s="2"/>
+      <c r="B250" s="2" t="s">
+        <v>749</v>
+      </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B251" s="2"/>
+      <c r="B251" s="2" t="s">
+        <v>750</v>
+      </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B252" s="2"/>
+      <c r="B252" s="2" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B253" s="2"/>
+      <c r="B253" s="2" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B254" s="2"/>
+      <c r="B254" s="2" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B255" s="2"/>
+      <c r="B255" s="2" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B256" s="2"/>
+      <c r="B256" s="2" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B257" s="2"/>
+      <c r="B257" s="2" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B258" s="2"/>
+      <c r="B258" s="2" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B259" s="2"/>
+      <c r="B259" s="2" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B260" s="2"/>
+      <c r="B260" s="2" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B261" s="2"/>
+      <c r="B261" s="2" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B262" s="2"/>
+      <c r="B262" s="2" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B263" s="2"/>
+      <c r="B263" s="2" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B264" s="2"/>
+      <c r="B264" s="2" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B265" s="2"/>
+      <c r="B265" s="2" t="s">
+        <v>764</v>
+      </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B266" s="2"/>
+      <c r="B266" s="2" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B267" s="2"/>
+      <c r="B267" s="2" t="s">
+        <v>766</v>
+      </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B268" s="2"/>
+      <c r="B268" s="2" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B269" s="2"/>
+      <c r="B269" s="2" t="s">
+        <v>768</v>
+      </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B270" s="2"/>
+      <c r="B270" s="2" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B271" s="2"/>
+      <c r="B271" s="2" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B272" s="2"/>
+      <c r="B272" s="2" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B273" s="2"/>
+      <c r="B273" s="2" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B274" s="2"/>
+      <c r="B274" s="2" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B275" s="2"/>
+      <c r="B275" s="2" t="s">
+        <v>774</v>
+      </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B276" s="2"/>
+      <c r="B276" s="2" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B277" s="2"/>
+      <c r="B277" s="2" t="s">
+        <v>776</v>
+      </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B278" s="2"/>
+      <c r="B278" s="2" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B279" s="2"/>
+      <c r="B279" s="2" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B280" s="2"/>
+      <c r="B280" s="2" t="s">
+        <v>779</v>
+      </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B281" s="2"/>
+      <c r="B281" s="2" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B282" s="2"/>
+      <c r="B282" s="2" t="s">
+        <v>781</v>
+      </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B283" s="2"/>
+      <c r="B283" s="2" t="s">
+        <v>782</v>
+      </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B284" s="2"/>
+      <c r="B284" s="2" t="s">
+        <v>783</v>
+      </c>
     </row>
     <row r="285" spans="1:2">
       <c r="A285" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B285" s="2"/>
+      <c r="B285" s="2" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B286" s="2"/>
+      <c r="B286" s="2" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="287" spans="1:2">
       <c r="A287" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B287" s="2"/>
+      <c r="B287" s="2" t="s">
+        <v>786</v>
+      </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B288" s="2"/>
+      <c r="B288" s="2" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B289" s="2"/>
+      <c r="B289" s="2" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="290" spans="1:2">
       <c r="A290" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B290" s="2"/>
+      <c r="B290" s="2" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="291" spans="1:2">
       <c r="A291" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B291" s="2"/>
+      <c r="B291" s="2" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="292" spans="1:2">
       <c r="A292" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B292" s="2"/>
+      <c r="B292" s="2" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="293" spans="1:2">
       <c r="A293" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B293" s="2"/>
+      <c r="B293" s="2" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="294" spans="1:2">
       <c r="A294" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="B294" s="2"/>
+      <c r="B294" s="2" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="295" spans="1:2">
       <c r="A295" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B295" s="2"/>
+      <c r="B295" s="2" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B296" s="2"/>
+      <c r="B296" s="2" t="s">
+        <v>795</v>
+      </c>
     </row>
     <row r="297" spans="1:2">
       <c r="A297" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B297" s="2"/>
+      <c r="B297" s="2" t="s">
+        <v>796</v>
+      </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="B298" s="2"/>
+      <c r="B298" s="2" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="299" spans="1:2">
       <c r="A299" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B299" s="2"/>
+      <c r="B299" s="2" t="s">
+        <v>798</v>
+      </c>
     </row>
     <row r="300" spans="1:2">
       <c r="A300" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="B300" s="2"/>
+      <c r="B300" s="2" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="301" spans="1:2">
       <c r="A301" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="B301" s="2"/>
+      <c r="B301" s="2" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="302" spans="1:2">
       <c r="A302" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B302" s="2"/>
+      <c r="B302" s="2" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="303" spans="1:2">
       <c r="A303" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="B303" s="2"/>
+      <c r="B303" s="2" t="s">
+        <v>802</v>
+      </c>
     </row>
     <row r="304" spans="1:2">
       <c r="A304" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="B304" s="2"/>
+      <c r="B304" s="2" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="305" spans="1:2">
       <c r="A305" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B305" s="2"/>
+      <c r="B305" s="2" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="306" spans="1:2">
       <c r="A306" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="B306" s="2"/>
+      <c r="B306" s="2" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="B307" s="2"/>
+      <c r="B307" s="2" t="s">
+        <v>806</v>
+      </c>
     </row>
     <row r="308" spans="1:2">
       <c r="A308" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B308" s="2"/>
+      <c r="B308" s="2" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="309" spans="1:2">
       <c r="A309" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="B309" s="2"/>
+      <c r="B309" s="2" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="310" spans="1:2">
       <c r="A310" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B310" s="2"/>
+      <c r="B310" s="2" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="311" spans="1:2">
       <c r="A311" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B311" s="2"/>
+      <c r="B311" s="2" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B312" s="2"/>
+      <c r="B312" s="2" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="313" spans="1:2">
       <c r="A313" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B313" s="2"/>
+      <c r="B313" s="2" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="314" spans="1:2">
       <c r="A314" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B314" s="2"/>
+      <c r="B314" s="2" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="315" spans="1:2">
       <c r="A315" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="B315" s="2"/>
+      <c r="B315" s="2" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="316" spans="1:2">
       <c r="A316" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="B316" s="2"/>
+      <c r="B316" s="2" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="317" spans="1:2">
       <c r="A317" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B317" s="2"/>
+      <c r="B317" s="2" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="318" spans="1:2">
       <c r="A318" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B318" s="2"/>
+      <c r="B318" s="2" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="319" spans="1:2">
       <c r="A319" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="B319" s="2"/>
+      <c r="B319" s="2" t="s">
+        <v>818</v>
+      </c>
     </row>
     <row r="320" spans="1:2">
       <c r="A320" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="B320" s="2"/>
+      <c r="B320" s="2" t="s">
+        <v>819</v>
+      </c>
     </row>
     <row r="321" spans="1:2">
       <c r="A321" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B321" s="2"/>
+      <c r="B321" s="2" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="322" spans="1:2">
       <c r="A322" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="B322" s="2"/>
+      <c r="B322" s="2" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="323" spans="1:2">
       <c r="A323" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="B323" s="2"/>
+      <c r="B323" s="2" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="324" spans="1:2">
       <c r="A324" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="B324" s="2"/>
+      <c r="B324" s="2" t="s">
+        <v>823</v>
+      </c>
     </row>
     <row r="325" spans="1:2">
       <c r="A325" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B325" s="2"/>
+      <c r="B325" s="2" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="326" spans="1:2">
       <c r="A326" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B326" s="2"/>
+      <c r="B326" s="2" t="s">
+        <v>825</v>
+      </c>
     </row>
     <row r="327" spans="1:2">
       <c r="A327" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="B327" s="2"/>
+      <c r="B327" s="2" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="328" spans="1:2">
       <c r="A328" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B328" s="2"/>
+      <c r="B328" s="2" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="329" spans="1:2">
       <c r="A329" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="B329" s="2"/>
+      <c r="B329" s="2" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="330" spans="1:2">
       <c r="A330" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B330" s="2"/>
+      <c r="B330" s="2" t="s">
+        <v>829</v>
+      </c>
     </row>
     <row r="331" spans="1:2">
       <c r="A331" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B331" s="2"/>
+      <c r="B331" s="2" t="s">
+        <v>830</v>
+      </c>
     </row>
     <row r="332" spans="1:2">
       <c r="A332" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="B332" s="2"/>
+      <c r="B332" s="2" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="333" spans="1:2">
       <c r="A333" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B333" s="2"/>
+      <c r="B333" s="2" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="334" spans="1:2">
       <c r="A334" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B334" s="2"/>
+      <c r="B334" s="2" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="335" spans="1:2">
       <c r="A335" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B335" s="2"/>
+      <c r="B335" s="2" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="336" spans="1:2">
       <c r="A336" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="B336" s="2"/>
+      <c r="B336" s="2" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="337" spans="1:2">
       <c r="A337" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="B337" s="2"/>
+      <c r="B337" s="2" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="338" spans="1:2">
       <c r="A338" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="B338" s="2"/>
+      <c r="B338" s="2" t="s">
+        <v>837</v>
+      </c>
     </row>
     <row r="339" spans="1:2">
       <c r="A339" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="B339" s="2"/>
+      <c r="B339" s="2" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="340" spans="1:2">
       <c r="A340" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="B340" s="2"/>
+      <c r="B340" s="2" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="341" spans="1:2">
       <c r="A341" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="B341" s="2"/>
+      <c r="B341" s="2" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="342" spans="1:2">
       <c r="A342" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="B342" s="2"/>
+      <c r="B342" s="2" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="343" spans="1:2">
       <c r="A343" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B343" s="2"/>
+      <c r="B343" s="2" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="344" spans="1:2">
       <c r="A344" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="B344" s="2"/>
+      <c r="B344" s="2" t="s">
+        <v>843</v>
+      </c>
     </row>
     <row r="345" spans="1:2">
       <c r="A345" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="B345" s="2"/>
+      <c r="B345" s="2" t="s">
+        <v>844</v>
+      </c>
     </row>
     <row r="346" spans="1:2">
       <c r="A346" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="B346" s="2"/>
+      <c r="B346" s="2" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="347" spans="1:2">
       <c r="A347" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="B347" s="2"/>
+      <c r="B347" s="2" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="348" spans="1:2">
       <c r="A348" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B348" s="2"/>
+      <c r="B348" s="2" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="349" spans="1:2">
       <c r="A349" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="B349" s="2"/>
+      <c r="B349" s="2" t="s">
+        <v>848</v>
+      </c>
     </row>
     <row r="350" spans="1:2">
       <c r="A350" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="B350" s="2"/>
+      <c r="B350" s="2" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="351" spans="1:2">
       <c r="A351" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="B351" s="2"/>
+      <c r="B351" s="2" t="s">
+        <v>850</v>
+      </c>
     </row>
     <row r="352" spans="1:2">
       <c r="A352" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B352" s="2"/>
+      <c r="B352" s="2" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="353" spans="1:2">
       <c r="A353" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="B353" s="2"/>
+      <c r="B353" s="2" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="354" spans="1:2">
       <c r="A354" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B354" s="2"/>
+      <c r="B354" s="2" t="s">
+        <v>853</v>
+      </c>
     </row>
     <row r="355" spans="1:2">
       <c r="A355" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="B355" s="2"/>
+      <c r="B355" s="2" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="356" spans="1:2">
       <c r="A356" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="B356" s="2"/>
+      <c r="B356" s="2" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="357" spans="1:2">
       <c r="A357" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="B357" s="2"/>
+      <c r="B357" s="2" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="358" spans="1:2">
       <c r="A358" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="B358" s="2"/>
+      <c r="B358" s="2" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="359" spans="1:2">
       <c r="A359" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B359" s="2"/>
+      <c r="B359" s="2" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="360" spans="1:2">
       <c r="A360" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="B360" s="2"/>
+      <c r="B360" s="2" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="361" spans="1:2">
       <c r="A361" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="B361" s="2"/>
+      <c r="B361" s="2" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="362" spans="1:2">
       <c r="A362" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="B362" s="2"/>
+      <c r="B362" s="2" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="363" spans="1:2">
       <c r="A363" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B363" s="2"/>
+      <c r="B363" s="2" t="s">
+        <v>862</v>
+      </c>
     </row>
     <row r="364" spans="1:2">
       <c r="A364" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="B364" s="2"/>
+      <c r="B364" s="2" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="365" spans="1:2">
       <c r="A365" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="B365" s="2"/>
+      <c r="B365" s="2" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="366" spans="1:2">
       <c r="A366" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="B366" s="2"/>
+      <c r="B366" s="2" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="367" spans="1:2">
       <c r="A367" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="B367" s="2"/>
+      <c r="B367" s="2" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="368" spans="1:2">
       <c r="A368" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="B368" s="2"/>
+      <c r="B368" s="2" t="s">
+        <v>867</v>
+      </c>
     </row>
     <row r="369" spans="1:2">
       <c r="A369" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="B369" s="2"/>
+      <c r="B369" s="2" t="s">
+        <v>868</v>
+      </c>
     </row>
     <row r="370" spans="1:2">
       <c r="A370" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B370" s="2"/>
+      <c r="B370" s="2" t="s">
+        <v>869</v>
+      </c>
     </row>
     <row r="371" spans="1:2">
       <c r="A371" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="B371" s="2"/>
+      <c r="B371" s="2" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="372" spans="1:2">
       <c r="A372" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="B372" s="2"/>
+      <c r="B372" s="2" t="s">
+        <v>871</v>
+      </c>
     </row>
     <row r="373" spans="1:2">
       <c r="A373" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="B373" s="2"/>
+      <c r="B373" s="2" t="s">
+        <v>872</v>
+      </c>
     </row>
     <row r="374" spans="1:2">
       <c r="A374" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="B374" s="2"/>
+      <c r="B374" s="2" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="375" spans="1:2">
       <c r="A375" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="B375" s="2"/>
+      <c r="B375" s="2" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="376" spans="1:2">
       <c r="A376" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="B376" s="2"/>
+      <c r="B376" s="2" t="s">
+        <v>875</v>
+      </c>
     </row>
     <row r="377" spans="1:2">
       <c r="A377" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="B377" s="2"/>
+      <c r="B377" s="2" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="378" spans="1:2">
       <c r="A378" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="B378" s="2"/>
+      <c r="B378" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="379" spans="1:2">
       <c r="A379" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="B379" s="2"/>
+      <c r="B379" s="2" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="380" spans="1:2">
       <c r="A380" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B380" s="2"/>
+      <c r="B380" s="2" t="s">
+        <v>879</v>
+      </c>
     </row>
     <row r="381" spans="1:2">
       <c r="A381" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="B381" s="2"/>
+      <c r="B381" s="2" t="s">
+        <v>880</v>
+      </c>
     </row>
     <row r="382" spans="1:2">
       <c r="A382" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B382" s="2"/>
+      <c r="B382" s="2" t="s">
+        <v>881</v>
+      </c>
     </row>
     <row r="383" spans="1:2">
       <c r="A383" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="B383" s="2"/>
+      <c r="B383" s="2" t="s">
+        <v>882</v>
+      </c>
     </row>
     <row r="384" spans="1:2">
       <c r="A384" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="B384" s="2"/>
+      <c r="B384" s="2" t="s">
+        <v>883</v>
+      </c>
     </row>
     <row r="385" spans="1:2">
       <c r="A385" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="B385" s="2"/>
+      <c r="B385" s="2" t="s">
+        <v>884</v>
+      </c>
     </row>
     <row r="386" spans="1:2">
       <c r="A386" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="B386" s="2"/>
+      <c r="B386" s="2" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="387" spans="1:2">
       <c r="A387" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="B387" s="2"/>
+      <c r="B387" s="2" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="388" spans="1:2">
       <c r="A388" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="B388" s="2"/>
+      <c r="B388" s="2" t="s">
+        <v>887</v>
+      </c>
     </row>
     <row r="389" spans="1:2">
       <c r="A389" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="B389" s="2"/>
+      <c r="B389" s="2" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="390" spans="1:2">
       <c r="A390" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="B390" s="2"/>
+      <c r="B390" s="2" t="s">
+        <v>889</v>
+      </c>
     </row>
     <row r="391" spans="1:2">
       <c r="A391" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="B391" s="2"/>
+      <c r="B391" s="2" t="s">
+        <v>890</v>
+      </c>
     </row>
     <row r="392" spans="1:2">
       <c r="A392" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="B392" s="2"/>
+      <c r="B392" s="2" t="s">
+        <v>891</v>
+      </c>
     </row>
     <row r="393" spans="1:2">
       <c r="A393" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="B393" s="2"/>
+      <c r="B393" s="2" t="s">
+        <v>892</v>
+      </c>
     </row>
     <row r="394" spans="1:2">
       <c r="A394" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B394" s="2"/>
+      <c r="B394" s="2" t="s">
+        <v>893</v>
+      </c>
     </row>
     <row r="395" spans="1:2">
       <c r="A395" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="B395" s="2"/>
+      <c r="B395" s="2" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="396" spans="1:2">
       <c r="A396" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="B396" s="2"/>
+      <c r="B396" s="2" t="s">
+        <v>895</v>
+      </c>
     </row>
     <row r="397" spans="1:2">
       <c r="A397" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="B397" s="2"/>
+      <c r="B397" s="2" t="s">
+        <v>896</v>
+      </c>
     </row>
     <row r="398" spans="1:2">
       <c r="A398" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="B398" s="2"/>
+      <c r="B398" s="2" t="s">
+        <v>897</v>
+      </c>
     </row>
     <row r="399" spans="1:2">
       <c r="A399" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="B399" s="2"/>
+      <c r="B399" s="2" t="s">
+        <v>898</v>
+      </c>
     </row>
     <row r="400" spans="1:2">
       <c r="A400" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="B400" s="2"/>
+      <c r="B400" s="2" t="s">
+        <v>899</v>
+      </c>
     </row>
     <row r="401" spans="1:2">
       <c r="A401" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="B401" s="2"/>
+      <c r="B401" s="2" t="s">
+        <v>900</v>
+      </c>
     </row>
     <row r="402" spans="1:2">
       <c r="A402" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="B402" s="2"/>
+      <c r="B402" s="2" t="s">
+        <v>901</v>
+      </c>
     </row>
     <row r="403" spans="1:2">
       <c r="A403" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="B403" s="2"/>
+      <c r="B403" s="2" t="s">
+        <v>902</v>
+      </c>
     </row>
     <row r="404" spans="1:2">
       <c r="A404" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="B404" s="2"/>
+      <c r="B404" s="2" t="s">
+        <v>903</v>
+      </c>
     </row>
     <row r="405" spans="1:2">
       <c r="A405" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="B405" s="2"/>
+      <c r="B405" s="2" t="s">
+        <v>904</v>
+      </c>
     </row>
     <row r="406" spans="1:2">
       <c r="A406" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="B406" s="2"/>
+      <c r="B406" s="2" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="407" spans="1:2">
       <c r="A407" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="B407" s="2"/>
+      <c r="B407" s="2" t="s">
+        <v>906</v>
+      </c>
     </row>
     <row r="408" spans="1:2">
       <c r="A408" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="B408" s="2"/>
+      <c r="B408" s="2" t="s">
+        <v>907</v>
+      </c>
     </row>
     <row r="409" spans="1:2">
       <c r="A409" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="B409" s="2"/>
+      <c r="B409" s="2" t="s">
+        <v>908</v>
+      </c>
     </row>
     <row r="410" spans="1:2">
       <c r="A410" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="B410" s="2"/>
+      <c r="B410" s="2" t="s">
+        <v>909</v>
+      </c>
     </row>
     <row r="411" spans="1:2">
       <c r="A411" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="B411" s="2"/>
+      <c r="B411" s="2" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="412" spans="1:2">
       <c r="A412" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="B412" s="2"/>
+      <c r="B412" s="2" t="s">
+        <v>911</v>
+      </c>
     </row>
     <row r="413" spans="1:2">
       <c r="A413" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="B413" s="2"/>
+      <c r="B413" s="2" t="s">
+        <v>912</v>
+      </c>
     </row>
     <row r="414" spans="1:2">
       <c r="A414" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="B414" s="2"/>
+      <c r="B414" s="2" t="s">
+        <v>913</v>
+      </c>
     </row>
     <row r="415" spans="1:2">
       <c r="A415" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="B415" s="2"/>
+      <c r="B415" s="2" t="s">
+        <v>914</v>
+      </c>
     </row>
     <row r="416" spans="1:2">
       <c r="A416" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="B416" s="2"/>
+      <c r="B416" s="2" t="s">
+        <v>915</v>
+      </c>
     </row>
     <row r="417" spans="1:2">
       <c r="A417" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="B417" s="2"/>
+      <c r="B417" s="2" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="418" spans="1:2">
       <c r="A418" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="B418" s="2"/>
+      <c r="B418" s="2" t="s">
+        <v>917</v>
+      </c>
     </row>
     <row r="419" spans="1:2">
       <c r="A419" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="B419" s="2"/>
+      <c r="B419" s="2" t="s">
+        <v>918</v>
+      </c>
     </row>
     <row r="420" spans="1:2">
       <c r="A420" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="B420" s="2"/>
+      <c r="B420" s="2" t="s">
+        <v>919</v>
+      </c>
     </row>
     <row r="421" spans="1:2">
       <c r="A421" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="B421" s="2"/>
+      <c r="B421" s="2" t="s">
+        <v>920</v>
+      </c>
     </row>
     <row r="422" spans="1:2">
       <c r="A422" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="B422" s="2"/>
+      <c r="B422" s="2" t="s">
+        <v>921</v>
+      </c>
     </row>
     <row r="423" spans="1:2">
       <c r="A423" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="B423" s="2"/>
+      <c r="B423" s="2" t="s">
+        <v>922</v>
+      </c>
     </row>
     <row r="424" spans="1:2">
       <c r="A424" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B424" s="2"/>
+      <c r="B424" s="2" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="425" spans="1:2">
       <c r="A425" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="B425" s="2"/>
+      <c r="B425" s="2" t="s">
+        <v>924</v>
+      </c>
     </row>
     <row r="426" spans="1:2">
       <c r="A426" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="B426" s="2"/>
+      <c r="B426" s="2" t="s">
+        <v>925</v>
+      </c>
     </row>
     <row r="427" spans="1:2">
       <c r="A427" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="B427" s="2"/>
+      <c r="B427" s="2" t="s">
+        <v>926</v>
+      </c>
     </row>
     <row r="428" spans="1:2">
       <c r="A428" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="B428" s="2"/>
+      <c r="B428" s="2" t="s">
+        <v>927</v>
+      </c>
     </row>
     <row r="429" spans="1:2">
       <c r="A429" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="B429" s="2"/>
+      <c r="B429" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
     <row r="430" spans="1:2">
       <c r="A430" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="B430" s="2"/>
+      <c r="B430" s="2" t="s">
+        <v>929</v>
+      </c>
     </row>
     <row r="431" spans="1:2">
       <c r="A431" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="B431" s="2"/>
+      <c r="B431" s="2" t="s">
+        <v>930</v>
+      </c>
     </row>
     <row r="432" spans="1:2">
       <c r="A432" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="B432" s="2"/>
+      <c r="B432" s="2" t="s">
+        <v>931</v>
+      </c>
     </row>
     <row r="433" spans="1:2">
       <c r="A433" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="B433" s="2"/>
+      <c r="B433" s="2" t="s">
+        <v>932</v>
+      </c>
     </row>
     <row r="434" spans="1:2">
       <c r="A434" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="B434" s="2"/>
+      <c r="B434" s="2" t="s">
+        <v>933</v>
+      </c>
     </row>
     <row r="435" spans="1:2">
       <c r="A435" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="B435" s="2"/>
+      <c r="B435" s="2" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="436" spans="1:2">
       <c r="A436" s="2" t="s">
@@ -6413,7 +7563,6 @@
       <c r="B501" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>